<commit_message>
data analysis graphs moving average works with 0 size queue
</commit_message>
<xml_diff>
--- a/rssi_data.xlsx
+++ b/rssi_data.xlsx
@@ -4010,10 +4010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F89"/>
+  <dimension ref="B1:F135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="93" workbookViewId="0">
-      <selection activeCell="B89" sqref="B44:B89"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="93" workbookViewId="0">
+      <selection activeCell="K94" sqref="K94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4891,7 +4891,7 @@
         <v>-87.227272727272705</v>
       </c>
       <c r="C66">
-        <f t="shared" ref="C66:C89" si="2">-B66</f>
+        <f t="shared" ref="C66:C129" si="2">-B66</f>
         <v>87.227272727272705</v>
       </c>
       <c r="D66">
@@ -5268,6 +5268,420 @@
       </c>
       <c r="F89">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B90">
+        <v>-64.44</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="2"/>
+        <v>64.44</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B91">
+        <v>-72</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B92">
+        <v>-77.272727272727195</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="2"/>
+        <v>77.272727272727195</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B93">
+        <v>-81.9583333333333</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="2"/>
+        <v>81.9583333333333</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B94">
+        <v>-81.521739130434696</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="2"/>
+        <v>81.521739130434696</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B95">
+        <v>-81.185185185185105</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="2"/>
+        <v>81.185185185185105</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B96">
+        <v>-82.588235294117595</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="2"/>
+        <v>82.588235294117595</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B97">
+        <v>-80.941176470588204</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="2"/>
+        <v>80.941176470588204</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B98">
+        <v>-81.260869565217305</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="2"/>
+        <v>81.260869565217305</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B99">
+        <v>-84.476190476190396</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="2"/>
+        <v>84.476190476190396</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B100">
+        <v>-83.210526315789394</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="2"/>
+        <v>83.210526315789394</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B101">
+        <v>-83.363636363636303</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="2"/>
+        <v>83.363636363636303</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B102">
+        <v>-83.35</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="2"/>
+        <v>83.35</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B103">
+        <v>-87.7777777777777</v>
+      </c>
+      <c r="C103">
+        <f t="shared" si="2"/>
+        <v>87.7777777777777</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B104">
+        <v>-86.142857142857096</v>
+      </c>
+      <c r="C104">
+        <f t="shared" si="2"/>
+        <v>86.142857142857096</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B105">
+        <v>-83.133333333333297</v>
+      </c>
+      <c r="C105">
+        <f t="shared" si="2"/>
+        <v>83.133333333333297</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B106">
+        <v>-85.052631578947299</v>
+      </c>
+      <c r="C106">
+        <f t="shared" si="2"/>
+        <v>85.052631578947299</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B107">
+        <v>-86</v>
+      </c>
+      <c r="C107">
+        <f t="shared" si="2"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B108">
+        <v>-90.75</v>
+      </c>
+      <c r="C108">
+        <f t="shared" si="2"/>
+        <v>90.75</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B109">
+        <v>-90.625</v>
+      </c>
+      <c r="C109">
+        <f t="shared" si="2"/>
+        <v>90.625</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B110">
+        <v>-85.823529411764696</v>
+      </c>
+      <c r="C110">
+        <f t="shared" si="2"/>
+        <v>85.823529411764696</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B111">
+        <v>-84.947368421052602</v>
+      </c>
+      <c r="C111">
+        <f t="shared" si="2"/>
+        <v>84.947368421052602</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B112">
+        <v>-84.315789473684205</v>
+      </c>
+      <c r="C112">
+        <f t="shared" si="2"/>
+        <v>84.315789473684205</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B113">
+        <v>-83.608695652173907</v>
+      </c>
+      <c r="C113">
+        <f t="shared" si="2"/>
+        <v>83.608695652173907</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B114">
+        <v>-83.875</v>
+      </c>
+      <c r="C114">
+        <f t="shared" si="2"/>
+        <v>83.875</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B115">
+        <v>-85.2222222222222</v>
+      </c>
+      <c r="C115">
+        <f t="shared" si="2"/>
+        <v>85.2222222222222</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B116">
+        <v>-85.625</v>
+      </c>
+      <c r="C116">
+        <f t="shared" si="2"/>
+        <v>85.625</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B117">
+        <v>-85.052631578947299</v>
+      </c>
+      <c r="C117">
+        <f t="shared" si="2"/>
+        <v>85.052631578947299</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B118">
+        <v>-85.052631578947299</v>
+      </c>
+      <c r="C118">
+        <f t="shared" si="2"/>
+        <v>85.052631578947299</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B119">
+        <v>-83.636363636363598</v>
+      </c>
+      <c r="C119">
+        <f t="shared" si="2"/>
+        <v>83.636363636363598</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B120">
+        <v>-84.047619047618994</v>
+      </c>
+      <c r="C120">
+        <f t="shared" si="2"/>
+        <v>84.047619047618994</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B121">
+        <v>-85.235294117647001</v>
+      </c>
+      <c r="C121">
+        <f t="shared" si="2"/>
+        <v>85.235294117647001</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B122">
+        <v>-90.125</v>
+      </c>
+      <c r="C122">
+        <f t="shared" si="2"/>
+        <v>90.125</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B123">
+        <v>-90.6666666666666</v>
+      </c>
+      <c r="C123">
+        <f t="shared" si="2"/>
+        <v>90.6666666666666</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B124">
+        <v>-83.894736842105203</v>
+      </c>
+      <c r="C124">
+        <f t="shared" si="2"/>
+        <v>83.894736842105203</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B125">
+        <v>-82.411764705882305</v>
+      </c>
+      <c r="C125">
+        <f t="shared" si="2"/>
+        <v>82.411764705882305</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B126">
+        <v>-85.461538461538396</v>
+      </c>
+      <c r="C126">
+        <f t="shared" si="2"/>
+        <v>85.461538461538396</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B127">
+        <v>-86.6875</v>
+      </c>
+      <c r="C127">
+        <f t="shared" si="2"/>
+        <v>86.6875</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B128">
+        <v>-78.117647058823493</v>
+      </c>
+      <c r="C128">
+        <f t="shared" si="2"/>
+        <v>78.117647058823493</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B129">
+        <v>-77.294117647058798</v>
+      </c>
+      <c r="C129">
+        <f t="shared" si="2"/>
+        <v>77.294117647058798</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B130">
+        <v>-87.0625</v>
+      </c>
+      <c r="C130">
+        <f t="shared" ref="C130:C135" si="3">-B130</f>
+        <v>87.0625</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B131">
+        <v>-89.6666666666666</v>
+      </c>
+      <c r="C131">
+        <f t="shared" si="3"/>
+        <v>89.6666666666666</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B132">
+        <v>-90.125</v>
+      </c>
+      <c r="C132">
+        <f t="shared" si="3"/>
+        <v>90.125</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B133">
+        <v>-85.636363636363598</v>
+      </c>
+      <c r="C133">
+        <f t="shared" si="3"/>
+        <v>85.636363636363598</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B134">
+        <v>-85.0625</v>
+      </c>
+      <c r="C134">
+        <f t="shared" si="3"/>
+        <v>85.0625</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B135">
+        <v>-93.5</v>
+      </c>
+      <c r="C135">
+        <f t="shared" si="3"/>
+        <v>93.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>